<commit_message>
RGH and Exo70F1 gene family analysis
</commit_message>
<xml_diff>
--- a/data/aegilops_tauschii_genomic_resources.xlsx
+++ b/data/aegilops_tauschii_genomic_resources.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -599,7 +599,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>